<commit_message>
Fixed : Student flow completed rename all files
</commit_message>
<xml_diff>
--- a/src/test/resources/Excel/FeedBackExcel.xlsx
+++ b/src/test/resources/Excel/FeedBackExcel.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>FeedbackName</t>
   </si>
@@ -36,6 +36,9 @@
   </si>
   <si>
     <t>Feedback Level automation4116</t>
+  </si>
+  <si>
+    <t>Feedback Level automation4222</t>
   </si>
 </sst>
 </file>
@@ -977,7 +980,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1003,6 +1006,11 @@
         <v>2</v>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>

</xml_diff>